<commit_message>
on the way to bless
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532772A5-E035-4758-B89D-B9D2F9AED861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99607E8-6196-4F91-94C4-69831A331282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="373">
   <si>
     <t>Sheet</t>
   </si>
@@ -1460,6 +1460,9 @@
   </si>
   <si>
     <t>ASI Master</t>
+  </si>
+  <si>
+    <t>Trololol</t>
   </si>
 </sst>
 </file>
@@ -2753,364 +2756,7 @@
     <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Percent 2 2" xfId="9" xr:uid="{EF7A7829-79FD-4611-956F-3356E04BECF0}"/>
   </cellStyles>
-  <dxfs count="265">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
+  <dxfs count="297">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3153,6 +2799,302 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5363,6 +5305,363 @@
         <color rgb="FF000000"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -5978,43 +6277,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="296" headerRowBorderDxfId="295" tableBorderDxfId="294" headerRowCellStyle="Normal 2">
   <autoFilter ref="B3:C14" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="293"/>
+    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="292"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="291" dataDxfId="289" headerRowBorderDxfId="290" tableBorderDxfId="288" headerRowCellStyle="Normal 2">
   <autoFilter ref="E3:F7" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="287"/>
+    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="286"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="285" tableBorderDxfId="284">
   <autoFilter ref="H3:I7" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="283"/>
+    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="282"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K6" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="K3:K6" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="281" tableBorderDxfId="280">
+  <autoFilter ref="K3:K7" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="279"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6607,52 +6906,52 @@
     <mergeCell ref="B32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="D6 D8:D9 F10 B4:F5 B11:F11 D12:F12">
-    <cfRule type="cellIs" dxfId="264" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="278" priority="8" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B10 B12">
-    <cfRule type="cellIs" dxfId="263" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="277" priority="14" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 C12">
-    <cfRule type="cellIs" dxfId="262" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="276" priority="15" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="cellIs" dxfId="261" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="275" priority="17" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F9">
-    <cfRule type="cellIs" dxfId="260" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="18" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="259" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="6" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="258" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="272" priority="4" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="257" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="271" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="256" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="270" priority="2" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="255" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6665,10 +6964,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFACB9E1-9EA9-4AE0-9315-1B70463FCABE}">
   <sheetPr codeName="Blad12"/>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7238,6 +7537,86 @@
       <c r="S19" s="59"/>
       <c r="T19" s="59"/>
     </row>
+    <row r="20" spans="1:20" ht="15.75">
+      <c r="A20" s="54" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" s="120" t="s">
+        <v>322</v>
+      </c>
+      <c r="C20" s="120" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="57"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="58" t="s">
+        <v>364</v>
+      </c>
+      <c r="B21" s="120" t="s">
+        <v>322</v>
+      </c>
+      <c r="C21" s="60"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="58" t="s">
+        <v>365</v>
+      </c>
+      <c r="B22" s="120" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="59"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="D3:H3"/>
@@ -7250,204 +7629,302 @@
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="T3:T4"/>
   </mergeCells>
-  <conditionalFormatting sqref="P6:T9 D7:H9 J6:N9 P11:S12 J11:N12 D11:H12 B5:B19">
-    <cfRule type="cellIs" dxfId="83" priority="313" operator="equal">
+  <conditionalFormatting sqref="P6:T9 D7:H9 J6:N9 P11:S12 J11:N12 D11:H12 B5:B22">
+    <cfRule type="cellIs" dxfId="97" priority="345" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="314" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="346" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="315" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="347" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="316" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="348" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="cellIs" dxfId="79" priority="321" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="353" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="322" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="354" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="323" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="355" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="324" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="356" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:H6">
-    <cfRule type="cellIs" dxfId="75" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="333" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="334" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="335" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="304" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="336" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:T19">
-    <cfRule type="cellIs" dxfId="71" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="141" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="142" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="143" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="144" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="cellIs" dxfId="67" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="153" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="154" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="155" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="156" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:H14">
-    <cfRule type="cellIs" dxfId="63" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="149" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="150" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="151" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="152" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15">
-    <cfRule type="cellIs" dxfId="59" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="145" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="146" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="147" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="148" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:H19">
-    <cfRule type="cellIs" dxfId="55" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="137" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="138" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="139" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="140" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:N19">
-    <cfRule type="cellIs" dxfId="51" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="133" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="134" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="135" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="136" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14:S19">
-    <cfRule type="cellIs" dxfId="47" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="129" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="130" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="131" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="132" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T11:T12">
-    <cfRule type="cellIs" dxfId="43" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="113" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="114" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="115" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="116" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="56" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="37" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T21">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:H21">
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T22">
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:H22">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:N22">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P21:S22">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+      <formula>"p"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B19" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B22" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
       <formula1>types_unit_phase_descr</formula1>
     </dataValidation>
   </dataValidations>
@@ -12061,44 +12538,44 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:I296">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J296">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>750</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>500</formula>
       <formula>749</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
       <formula>250</formula>
       <formula>499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="between">
       <formula>1</formula>
       <formula>249</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A296">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>NOT(ISERROR(SEARCH(" ",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B296">
-    <cfRule type="duplicateValues" dxfId="18" priority="278"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="278"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F296" xr:uid="{7E766BAA-3222-4A1B-96F6-6DD936D34E56}">
@@ -12120,7 +12597,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12200,7 +12677,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="118" t="s">
-        <v>199</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -12222,8 +12699,8 @@
       <c r="I5" s="112">
         <v>250</v>
       </c>
-      <c r="K5" s="119" t="s">
-        <v>360</v>
+      <c r="K5" s="118" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:11">
@@ -12246,7 +12723,7 @@
         <v>500</v>
       </c>
       <c r="K6" s="119" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1">
@@ -12267,6 +12744,9 @@
       </c>
       <c r="I7" s="114">
         <v>750</v>
+      </c>
+      <c r="K7" s="119" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -18582,42 +19062,42 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K293">
-    <cfRule type="cellIs" dxfId="254" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="250" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="duplicateValues" dxfId="249" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="248" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B293 B7:B8 B14:B50">
-    <cfRule type="duplicateValues" dxfId="247" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N293">
-    <cfRule type="cellIs" dxfId="246" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23957,86 +24437,86 @@
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="242" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="238" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="234" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="230" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="228" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K300">
-    <cfRule type="cellIs" dxfId="226" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8 B11:B14 B20:B300">
-    <cfRule type="duplicateValues" dxfId="222" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="221" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="220" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="219" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="33"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F19" xr:uid="{858AD274-EE67-43BB-A3F1-3780D7923764}">
@@ -27610,75 +28090,75 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F303">
-    <cfRule type="cellIs" dxfId="218" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G303">
-    <cfRule type="cellIs" dxfId="214" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H303">
-    <cfRule type="cellIs" dxfId="210" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I303">
-    <cfRule type="cellIs" dxfId="206" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B7 B9:B10 B12:B13 B15:B16 B18:B303">
-    <cfRule type="duplicateValues" dxfId="202" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="201" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="200" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="199" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="198" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="34"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31381,77 +31861,77 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="197" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="193" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="189" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:I300">
-    <cfRule type="cellIs" dxfId="185" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="181" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="177" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -36311,21 +36791,21 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I300">
-    <cfRule type="cellIs" dxfId="176" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="172" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -41181,157 +41661,157 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="171" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="167" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="163" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="159" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6 J15:J300">
-    <cfRule type="cellIs" dxfId="155" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B300">
-    <cfRule type="duplicateValues" dxfId="151" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="150" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="149" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="148" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="147" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="146" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="142" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="138" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="134" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="47" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="48" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="49" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="50" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J14">
-    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46999,21 +47479,21 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:J299">
-    <cfRule type="cellIs" dxfId="126" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B299">
-    <cfRule type="duplicateValues" dxfId="122" priority="273"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="273"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -51728,134 +52208,134 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="121" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="113" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6 I11:I300">
-    <cfRule type="cellIs" dxfId="109" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 B13:B300">
-    <cfRule type="duplicateValues" dxfId="105" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="104" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="103" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="102" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="101" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="100" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="31" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="32" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="33" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="96" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="92" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="88" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
First working version for units and phases
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2B90C3-540D-46F7-A5B2-C93EDAA71506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B331B5E-6AAC-4C03-8DF4-0C9EF5B889F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
@@ -2762,6 +2762,363 @@
   <dxfs count="293">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -5271,363 +5628,6 @@
         <color rgb="FF000000"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6243,43 +6243,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="292" headerRowBorderDxfId="291" tableBorderDxfId="290" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" headerRowCellStyle="Normal 2">
   <autoFilter ref="B3:C14" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="289"/>
-    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="288"/>
+    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="287" dataDxfId="285" headerRowBorderDxfId="286" tableBorderDxfId="284" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Normal 2">
   <autoFilter ref="E3:F7" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="283"/>
-    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="282"/>
+    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="281" tableBorderDxfId="280">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="H3:I7" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="279"/>
-    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="278"/>
+    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="277" tableBorderDxfId="276">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="K3:K7" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="275"/>
+    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6872,52 +6872,52 @@
     <mergeCell ref="B32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="D6 D8:D9 F10 B4:F5 B11:F11 D12:F12">
-    <cfRule type="cellIs" dxfId="274" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="292" priority="8" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B10 B12">
-    <cfRule type="cellIs" dxfId="273" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="291" priority="14" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 C12">
-    <cfRule type="cellIs" dxfId="272" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="290" priority="15" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="cellIs" dxfId="271" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="289" priority="17" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F9">
-    <cfRule type="cellIs" dxfId="270" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="288" priority="18" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="269" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="287" priority="6" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="268" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="286" priority="4" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="267" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="285" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="266" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="284" priority="2" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="265" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="283" priority="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6933,7 +6933,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7535,7 +7535,7 @@
         <v>370</v>
       </c>
       <c r="B20" s="120" t="s">
-        <v>322</v>
+        <v>372</v>
       </c>
       <c r="C20" s="120"/>
       <c r="D20" s="120" t="s">
@@ -7626,300 +7626,300 @@
     <mergeCell ref="U3:U4"/>
   </mergeCells>
   <conditionalFormatting sqref="Q6:U9 E7:I9 K6:O9 Q11:T12 K11:O12 E11:I12 B20:C22 B5:B19">
-    <cfRule type="cellIs" dxfId="93" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="345" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="346" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="347" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="348" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6">
-    <cfRule type="cellIs" dxfId="89" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="353" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="354" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="355" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="355" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="356" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="356" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:I6">
-    <cfRule type="cellIs" dxfId="85" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="333" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="334" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="334" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="335" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="335" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="336" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:U19">
-    <cfRule type="cellIs" dxfId="81" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="141" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="142" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="143" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="144" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="77" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="153" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="154" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="155" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="156" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:I14">
-    <cfRule type="cellIs" dxfId="73" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="149" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="150" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="151" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="152" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15">
-    <cfRule type="cellIs" dxfId="69" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="145" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="146" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="147" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="148" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:I19">
-    <cfRule type="cellIs" dxfId="65" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="137" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="138" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="139" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="140" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:O19">
-    <cfRule type="cellIs" dxfId="61" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="133" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="134" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="135" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="136" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:T19">
-    <cfRule type="cellIs" dxfId="57" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="129" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="130" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="131" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="132" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:U12">
-    <cfRule type="cellIs" dxfId="53" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="113" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="114" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="115" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="116" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="53" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="54" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="42" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="43" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="44" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U21">
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="32" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:I21">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="28" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:I22">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="14" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21:O22">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q21:T22">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B22 C20:C22" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
       <formula1>types_unit_phase_descr</formula1>
     </dataValidation>
@@ -12534,44 +12534,44 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:I296">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J296">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="between">
       <formula>750</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
       <formula>500</formula>
       <formula>749</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="between">
       <formula>250</formula>
       <formula>499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="between">
       <formula>1</formula>
       <formula>249</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A296">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>NOT(ISERROR(SEARCH(" ",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B296">
-    <cfRule type="duplicateValues" dxfId="0" priority="278"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="278"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F296" xr:uid="{7E766BAA-3222-4A1B-96F6-6DD936D34E56}">
@@ -19058,42 +19058,42 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K293">
-    <cfRule type="cellIs" dxfId="264" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="261" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="260" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="278" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="duplicateValues" dxfId="259" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="277" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="258" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="276" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B293 B7:B8 B14:B50">
-    <cfRule type="duplicateValues" dxfId="257" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="275" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N293">
-    <cfRule type="cellIs" dxfId="256" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24433,86 +24433,86 @@
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="252" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="249" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="248" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="246" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="244" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="240" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K300">
-    <cfRule type="cellIs" dxfId="236" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8 B11:B14 B20:B300">
-    <cfRule type="duplicateValues" dxfId="232" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="231" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="230" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="229" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="33"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F19" xr:uid="{858AD274-EE67-43BB-A3F1-3780D7923764}">
@@ -28086,75 +28086,75 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F303">
-    <cfRule type="cellIs" dxfId="228" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="225" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G303">
-    <cfRule type="cellIs" dxfId="224" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H303">
-    <cfRule type="cellIs" dxfId="220" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I303">
-    <cfRule type="cellIs" dxfId="216" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B7 B9:B10 B12:B13 B15:B16 B18:B303">
-    <cfRule type="duplicateValues" dxfId="212" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="211" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="210" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="209" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="208" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="34"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31857,77 +31857,77 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="207" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="203" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="199" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:I300">
-    <cfRule type="cellIs" dxfId="195" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="191" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="187" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -36787,21 +36787,21 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I300">
-    <cfRule type="cellIs" dxfId="186" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="182" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -41657,157 +41657,157 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="181" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="177" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="173" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="169" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6 J15:J300">
-    <cfRule type="cellIs" dxfId="165" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B300">
-    <cfRule type="duplicateValues" dxfId="161" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="160" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="159" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="158" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="157" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="156" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="152" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="148" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="144" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="47" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="48" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="49" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="50" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J14">
-    <cfRule type="cellIs" dxfId="140" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47477,21 +47477,21 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:J299">
-    <cfRule type="cellIs" dxfId="136" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B299">
-    <cfRule type="duplicateValues" dxfId="132" priority="273"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="273"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -52206,134 +52206,134 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="131" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="127" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="123" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6 I11:I300">
-    <cfRule type="cellIs" dxfId="119" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 B13:B300">
-    <cfRule type="duplicateValues" dxfId="115" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="114" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="113" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="112" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="111" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="110" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="31" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="32" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="33" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="106" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="102" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="98" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
first working clean version, and with cp1252
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B331B5E-6AAC-4C03-8DF4-0C9EF5B889F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41EAECA-74D7-4815-8F5C-DE521CED1874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="372">
   <si>
     <t>Sheet</t>
   </si>
@@ -1456,16 +1456,10 @@
     <t>ASI Master</t>
   </si>
   <si>
-    <t>Trololol</t>
-  </si>
-  <si>
     <t>Line_Unit</t>
   </si>
   <si>
     <t>Tank_Unit</t>
-  </si>
-  <si>
-    <t>PLClol</t>
   </si>
 </sst>
 </file>
@@ -2760,363 +2754,6 @@
     <cellStyle name="Percent 2 2" xfId="9" xr:uid="{EF7A7829-79FD-4611-956F-3356E04BECF0}"/>
   </cellStyles>
   <dxfs count="293">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Trade gothic"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F8F8"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5628,6 +5265,363 @@
         <color rgb="FF000000"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Trade gothic"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F8F8"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6243,43 +6237,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}" name="valve_configs_table" displayName="valve_configs_table" ref="B3:C14" totalsRowShown="0" headerRowDxfId="292" headerRowBorderDxfId="291" tableBorderDxfId="290" headerRowCellStyle="Normal 2">
   <autoFilter ref="B3:C14" xr:uid="{FE4667D9-ACA3-4782-A460-2796D1278DB5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{D2B99697-6C22-4A65-9A1B-E36D1780E905}" name="Description" dataDxfId="289"/>
+    <tableColumn id="2" xr3:uid="{0C7255C4-22B6-457A-870A-411B65308579}" name="Value" dataDxfId="288"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}" name="motor_configs_table" displayName="motor_configs_table" ref="E3:F7" totalsRowShown="0" headerRowDxfId="287" dataDxfId="285" headerRowBorderDxfId="286" tableBorderDxfId="284" headerRowCellStyle="Normal 2">
   <autoFilter ref="E3:F7" xr:uid="{CBF749F0-70C7-416D-BC61-9BB1660F2FE0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{3566CC7F-11CE-4C21-9EB5-FA275F790C03}" name="Description" dataDxfId="283"/>
+    <tableColumn id="2" xr3:uid="{7BD42503-42BD-4F3C-A5DC-32DAB0E6CD55}" name="Value" dataDxfId="282"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}" name="alarm_configs_table" displayName="alarm_configs_table" ref="H3:I7" totalsRowShown="0" headerRowBorderDxfId="281" tableBorderDxfId="280">
   <autoFilter ref="H3:I7" xr:uid="{CFAD691F-B503-4ED4-8D8B-83FE92D1647F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{708D6350-80FE-46FF-B9B2-EC74246F1C57}" name="Description" dataDxfId="279"/>
+    <tableColumn id="2" xr3:uid="{94C6C4A0-B062-49D6-9CCC-0CD2BD3F95A4}" name="Value" dataDxfId="278"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="277" tableBorderDxfId="276">
   <autoFilter ref="K3:K7" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="275"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6872,52 +6866,52 @@
     <mergeCell ref="B32:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="D6 D8:D9 F10 B4:F5 B11:F11 D12:F12">
-    <cfRule type="cellIs" dxfId="292" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="274" priority="8" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B10 B12">
-    <cfRule type="cellIs" dxfId="291" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="273" priority="14" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C10 C12">
-    <cfRule type="cellIs" dxfId="290" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="272" priority="15" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E9">
-    <cfRule type="cellIs" dxfId="289" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="271" priority="17" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F9">
-    <cfRule type="cellIs" dxfId="288" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="270" priority="18" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="287" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="269" priority="6" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="286" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="268" priority="4" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="285" priority="3" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="267" priority="3" stopIfTrue="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E7">
-    <cfRule type="cellIs" dxfId="284" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="266" priority="2" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="283" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="265" priority="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6930,10 +6924,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFACB9E1-9EA9-4AE0-9315-1B70463FCABE}">
   <sheetPr codeName="Blad12"/>
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7118,7 +7112,7 @@
         <v>357</v>
       </c>
       <c r="B5" s="120" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>84</v>
@@ -7257,7 +7251,7 @@
         <v>360</v>
       </c>
       <c r="B10" s="120" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>84</v>
@@ -7342,7 +7336,7 @@
         <v>361</v>
       </c>
       <c r="B13" s="120" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>226</v>
@@ -7530,89 +7524,6 @@
       <c r="T19" s="59"/>
       <c r="U19" s="59"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75">
-      <c r="A20" s="54" t="s">
-        <v>370</v>
-      </c>
-      <c r="B20" s="120" t="s">
-        <v>372</v>
-      </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120" t="s">
-        <v>373</v>
-      </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="57"/>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="58" t="s">
-        <v>362</v>
-      </c>
-      <c r="B21" s="120" t="s">
-        <v>322</v>
-      </c>
-      <c r="C21" s="120"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="59"/>
-      <c r="U21" s="59"/>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="58" t="s">
-        <v>363</v>
-      </c>
-      <c r="B22" s="120" t="s">
-        <v>322</v>
-      </c>
-      <c r="C22" s="120"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59"/>
-      <c r="T22" s="59"/>
-      <c r="U22" s="59"/>
-    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="E3:I3"/>
@@ -7625,302 +7536,204 @@
     <mergeCell ref="Q3:T3"/>
     <mergeCell ref="U3:U4"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q6:U9 E7:I9 K6:O9 Q11:T12 K11:O12 E11:I12 B20:C22 B5:B19">
-    <cfRule type="cellIs" dxfId="111" priority="345" operator="equal">
+  <conditionalFormatting sqref="Q6:U9 E7:I9 K6:O9 Q11:T12 K11:O12 E11:I12 B5:B19">
+    <cfRule type="cellIs" dxfId="93" priority="345" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="346" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="347" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="348" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U6">
-    <cfRule type="cellIs" dxfId="107" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="353" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="354" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="355" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="355" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="356" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="356" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:I6">
-    <cfRule type="cellIs" dxfId="103" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="333" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="334" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="334" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="335" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="335" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="336" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:U19">
-    <cfRule type="cellIs" dxfId="99" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="141" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="142" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="143" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="144" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="95" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="153" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="154" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="155" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="156" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:I14">
-    <cfRule type="cellIs" dxfId="91" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="149" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="150" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="151" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="152" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U15">
-    <cfRule type="cellIs" dxfId="87" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="145" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="146" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="147" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="148" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:I19">
-    <cfRule type="cellIs" dxfId="83" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="137" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="138" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="139" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="140" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:O19">
-    <cfRule type="cellIs" dxfId="79" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="133" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="134" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="135" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="136" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:T19">
-    <cfRule type="cellIs" dxfId="75" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="129" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="130" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="131" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="132" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:U12">
-    <cfRule type="cellIs" dxfId="71" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="113" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="114" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="115" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="116" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="67" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="63" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U21">
-    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="31" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="32" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:I21">
-    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="28" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U22">
-    <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:I22">
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="14" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="15" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="16" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:O22">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q21:T22">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
-      <formula>"P"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
-      <formula>"p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B22 C20:C22" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B19" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
       <formula1>types_unit_phase_descr</formula1>
     </dataValidation>
   </dataValidations>
@@ -12534,44 +12347,44 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:I296">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J296">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>750</formula>
       <formula>999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="between">
       <formula>500</formula>
       <formula>749</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="between">
       <formula>250</formula>
       <formula>499</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="between">
       <formula>1</formula>
       <formula>249</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A296">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>NOT(ISERROR(SEARCH(" ",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B296">
-    <cfRule type="duplicateValues" dxfId="18" priority="278"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="278"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F296" xr:uid="{7E766BAA-3222-4A1B-96F6-6DD936D34E56}">
@@ -12719,7 +12532,7 @@
         <v>500</v>
       </c>
       <c r="K6" s="119" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1">
@@ -12742,7 +12555,7 @@
         <v>750</v>
       </c>
       <c r="K7" s="119" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -19058,42 +18871,42 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K293">
-    <cfRule type="cellIs" dxfId="282" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="279" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="278" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="260" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="duplicateValues" dxfId="277" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="276" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:B293 B7:B8 B14:B50">
-    <cfRule type="duplicateValues" dxfId="275" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N293">
-    <cfRule type="cellIs" dxfId="274" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24433,86 +24246,86 @@
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="270" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="267" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="266" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="264" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="262" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="261" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="259" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="258" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K300">
-    <cfRule type="cellIs" dxfId="254" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8 B11:B14 B20:B300">
-    <cfRule type="duplicateValues" dxfId="250" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="249" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="248" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="247" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="33"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F19" xr:uid="{858AD274-EE67-43BB-A3F1-3780D7923764}">
@@ -28086,75 +27899,75 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F303">
-    <cfRule type="cellIs" dxfId="246" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G303">
-    <cfRule type="cellIs" dxfId="242" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H303">
-    <cfRule type="cellIs" dxfId="238" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I303">
-    <cfRule type="cellIs" dxfId="234" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B7 B9:B10 B12:B13 B15:B16 B18:B303">
-    <cfRule type="duplicateValues" dxfId="230" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="229" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="228" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="227" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="226" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="34"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31857,77 +31670,77 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="225" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="221" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="217" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:I300">
-    <cfRule type="cellIs" dxfId="213" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J300">
-    <cfRule type="cellIs" dxfId="209" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="205" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="30"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -36787,21 +36600,21 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I300">
-    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="200" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -41657,157 +41470,157 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="199" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="195" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="191" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="187" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6 J15:J300">
-    <cfRule type="cellIs" dxfId="183" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B300">
-    <cfRule type="duplicateValues" dxfId="179" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="178" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="177" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="176" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="175" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="174" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="170" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="166" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="162" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="47" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="48" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="49" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="50" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J14">
-    <cfRule type="cellIs" dxfId="158" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47477,21 +47290,21 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:J299">
-    <cfRule type="cellIs" dxfId="154" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B299">
-    <cfRule type="duplicateValues" dxfId="150" priority="273"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="273"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -52206,134 +52019,134 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="149" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="145" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="141" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="19" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="20" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="21" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6 I11:I300">
-    <cfRule type="cellIs" dxfId="137" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11 B13:B300">
-    <cfRule type="duplicateValues" dxfId="133" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="132" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="131" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="130" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="129" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="128" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="31" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="32" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="33" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="34" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="124" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="120" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="116" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add s7 parse func
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E86FEC-DCB2-419D-B659-72CBEDAF8E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB6EFD-DDAA-4ABE-BE9C-FC45048ED1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -2793,6 +2793,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="medium">
           <color auto="1"/>
         </left>
@@ -2803,13 +2810,6 @@
           <color auto="1"/>
         </top>
         <bottom style="medium">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
@@ -4122,6 +4122,53 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -4500,53 +4547,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6017,7 +6017,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
   <autoFilter ref="K3:K7" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="0"/>
@@ -6326,8 +6326,8 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:AMC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6689,7 +6689,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7510,7 +7510,9 @@
   <sheetPr codeName="Blad11"/>
   <dimension ref="A1:AMA296"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -7678,14 +7680,14 @@
         <v>85</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>335</v>
+        <v>4</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="74">
         <f>IF(ISBLANK(F7),"",VLOOKUP(F7,alarm_configs_table[],2,))</f>
-        <v>1</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -12167,8 +12169,8 @@
   </sheetPr>
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12399,7 +12401,7 @@
   <dimension ref="A1:ALK293"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -18672,7 +18674,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F62 F293" xr:uid="{CD348D37-DD25-4857-B38F-E4611E7771B6}">
       <formula1>valve_configs_descr</formula1>
     </dataValidation>
@@ -18692,7 +18694,9 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:ALU300"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -36358,157 +36362,157 @@
     <mergeCell ref="L2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:F300">
-    <cfRule type="cellIs" dxfId="171" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="7" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="9" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G300">
-    <cfRule type="cellIs" dxfId="167" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="11" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="12" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H300">
-    <cfRule type="cellIs" dxfId="163" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="16" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:I300">
-    <cfRule type="cellIs" dxfId="159" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="23" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="24" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="25" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6 J15:J300">
-    <cfRule type="cellIs" dxfId="155" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="27" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="28" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="29" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B300">
-    <cfRule type="duplicateValues" dxfId="151" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 B8">
-    <cfRule type="duplicateValues" dxfId="150" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="149" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="148" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="147" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="146" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="35" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="36" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="37" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="38" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="142" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="39" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="40" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="41" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="42" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="138" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="43" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="44" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="45" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="cellIs" dxfId="134" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="47" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="48" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="49" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="50" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J14">
-    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36523,7 +36527,9 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:AME300"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -41370,21 +41376,21 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:I300">
-    <cfRule type="cellIs" dxfId="176" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="3" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B300">
-    <cfRule type="duplicateValues" dxfId="172" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="26"/>
   </conditionalFormatting>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -41398,7 +41404,7 @@
   <dimension ref="A1:AMH299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -47079,7 +47085,9 @@
   <sheetPr codeName="Blad10"/>
   <dimension ref="A1:AMG300"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Add support for absolute s7-db and offset
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB6EFD-DDAA-4ABE-BE9C-FC45048ED1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA015F9F-872C-4248-B61F-71899B6FB081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="390">
   <si>
     <t>Sheet</t>
   </si>
@@ -1467,6 +1467,54 @@
   <si>
     <t>• Channge Phases sheet, more data for automation-boilerplate, now we can create Intouch taglist with the script. Add table in _configs sheet for Units and phases</t>
   </si>
+  <si>
+    <t>DB900.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB900.DBX52.0</t>
+  </si>
+  <si>
+    <t>DB900.DBX300.0</t>
+  </si>
+  <si>
+    <t>DB900.DBX400.0</t>
+  </si>
+  <si>
+    <t>DB900.DBX522.0</t>
+  </si>
+  <si>
+    <t>DB5100.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB5100.DBX300.0</t>
+  </si>
+  <si>
+    <t>DB5100.DBX400.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX0.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX52.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX300.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX400.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX722.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX822.0</t>
+  </si>
+  <si>
+    <t>DB1337.DBX922.0</t>
+  </si>
+  <si>
+    <t>DB_start_address</t>
+  </si>
 </sst>
 </file>
 
@@ -1475,7 +1523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1724,6 +1772,13 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2382,7 +2437,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2685,6 +2740,10 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="33" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2793,13 +2852,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color auto="1"/>
         </left>
@@ -2810,6 +2862,13 @@
           <color auto="1"/>
         </top>
         <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
@@ -6017,7 +6076,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}" name="types_unit_phase_table" displayName="types_unit_phase_table" ref="K3:K7" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="K3:K7" xr:uid="{87CC4E56-03D3-40F1-AEAA-382187738863}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F7F9DF1F-D2AD-4AD1-A84E-14353F41BEDC}" name="Description" dataDxfId="0"/>
@@ -6587,38 +6646,38 @@
       <c r="F12" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A31" s="127" t="s">
+      <c r="A31" s="129" t="s">
         <v>327</v>
       </c>
-      <c r="B31" s="128"/>
-      <c r="C31" s="128"/>
-      <c r="D31" s="128"/>
-      <c r="E31" s="128"/>
-      <c r="F31" s="129"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="131"/>
     </row>
     <row r="32" spans="1:6" ht="97.5" customHeight="1" thickBot="1">
       <c r="A32" s="98" t="s">
         <v>324</v>
       </c>
-      <c r="B32" s="130" t="s">
+      <c r="B32" s="132" t="s">
         <v>356</v>
       </c>
-      <c r="C32" s="131"/>
-      <c r="D32" s="131"/>
-      <c r="E32" s="131"/>
-      <c r="F32" s="132"/>
+      <c r="C32" s="133"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="134"/>
     </row>
     <row r="33" spans="1:6" ht="32.25" customHeight="1">
       <c r="A33" s="98" t="s">
         <v>372</v>
       </c>
-      <c r="B33" s="130" t="s">
+      <c r="B33" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="C33" s="131"/>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
-      <c r="F33" s="132"/>
+      <c r="C33" s="133"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="134"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:A12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -6686,26 +6745,27 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFACB9E1-9EA9-4AE0-9315-1B70463FCABE}">
   <sheetPr codeName="Blad12"/>
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" style="49" customWidth="1"/>
     <col min="2" max="4" width="12.7109375" style="49" customWidth="1"/>
-    <col min="5" max="9" width="10.7109375" style="49" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="49" customWidth="1"/>
-    <col min="11" max="15" width="10.7109375" style="49" customWidth="1"/>
-    <col min="16" max="16" width="4.7109375" style="49" customWidth="1"/>
-    <col min="17" max="20" width="10.7109375" style="49" customWidth="1"/>
-    <col min="21" max="21" width="18.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="49"/>
+    <col min="5" max="5" width="16.28515625" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="10.7109375" style="49" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="49" customWidth="1"/>
+    <col min="12" max="16" width="10.7109375" style="49" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" style="49" customWidth="1"/>
+    <col min="18" max="21" width="10.7109375" style="49" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:22" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="46"/>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -6719,22 +6779,23 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46"/>
-      <c r="N1" s="47"/>
+      <c r="N1" s="46"/>
       <c r="O1" s="47"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="136" t="str">
+      <c r="P1" s="47"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="138" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="S1" s="136"/>
-      <c r="T1" s="134" t="str">
+      <c r="T1" s="138"/>
+      <c r="U1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="U1" s="135"/>
-    </row>
-    <row r="2" spans="1:21" ht="18" customHeight="1">
+      <c r="V1" s="137"/>
+    </row>
+    <row r="2" spans="1:22" ht="18" customHeight="1">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
@@ -6748,69 +6809,71 @@
       <c r="K2" s="46"/>
       <c r="L2" s="46"/>
       <c r="M2" s="46"/>
-      <c r="N2" s="47"/>
+      <c r="N2" s="46"/>
       <c r="O2" s="47"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="136" t="str">
+      <c r="P2" s="47"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="138" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="S2" s="136"/>
-      <c r="T2" s="134" t="str">
+      <c r="T2" s="138"/>
+      <c r="U2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="U2" s="135"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="138" t="s">
+      <c r="V2" s="137"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="140" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="138" t="s">
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="140" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="138" t="s">
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="140" t="s">
         <v>197</v>
       </c>
-      <c r="L3" s="139" t="s">
+      <c r="M3" s="141" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="139" t="s">
+      <c r="N3" s="141" t="s">
         <v>197</v>
       </c>
-      <c r="N3" s="139" t="s">
+      <c r="O3" s="141" t="s">
         <v>197</v>
       </c>
-      <c r="O3" s="140" t="s">
+      <c r="P3" s="142" t="s">
         <v>197</v>
       </c>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="138" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="140" t="s">
         <v>198</v>
       </c>
-      <c r="R3" s="139" t="s">
+      <c r="S3" s="141" t="s">
         <v>198</v>
       </c>
-      <c r="S3" s="139" t="s">
+      <c r="T3" s="141" t="s">
         <v>198</v>
       </c>
-      <c r="T3" s="139" t="s">
+      <c r="U3" s="141" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="142" t="s">
+      <c r="V3" s="144" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="53" customFormat="1" ht="11.25" customHeight="1">
+    <row r="4" spans="1:22" s="53" customFormat="1" ht="11.25" customHeight="1">
       <c r="A4" s="121" t="s">
         <v>12</v>
       </c>
@@ -6823,53 +6886,56 @@
       <c r="D4" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="121" t="s">
+        <v>389</v>
+      </c>
+      <c r="F4" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="G4" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="H4" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="I4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="J4" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="J4" s="52"/>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="52"/>
+      <c r="L4" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="M4" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="M4" s="51" t="s">
+      <c r="N4" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="N4" s="51" t="s">
+      <c r="O4" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="O4" s="51" t="s">
+      <c r="P4" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52"/>
+      <c r="R4" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="R4" s="51" t="s">
+      <c r="S4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="51" t="s">
+      <c r="T4" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="T4" s="51" t="s">
+      <c r="U4" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="U4" s="143"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75">
+      <c r="V4" s="145"/>
+    </row>
+    <row r="5" spans="1:22" ht="15.75">
       <c r="A5" s="54" t="s">
         <v>357</v>
       </c>
@@ -6882,25 +6948,28 @@
       <c r="D5" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="55"/>
+      <c r="E5" s="128" t="s">
+        <v>374</v>
+      </c>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="55"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="55"/>
       <c r="M5" s="55"/>
       <c r="N5" s="55"/>
       <c r="O5" s="55"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="55"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="56"/>
       <c r="R5" s="55"/>
       <c r="S5" s="55"/>
       <c r="T5" s="55"/>
-      <c r="U5" s="57"/>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="U5" s="55"/>
+      <c r="V5" s="57"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="58" t="s">
         <v>314</v>
       </c>
@@ -6909,25 +6978,28 @@
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="128" t="s">
+        <v>375</v>
+      </c>
       <c r="F6" s="59"/>
       <c r="G6" s="59"/>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
       <c r="L6" s="59"/>
       <c r="M6" s="59"/>
       <c r="N6" s="59"/>
       <c r="O6" s="59"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="60"/>
       <c r="R6" s="59"/>
       <c r="S6" s="59"/>
       <c r="T6" s="59"/>
       <c r="U6" s="59"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="59"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="58" t="s">
         <v>145</v>
       </c>
@@ -6936,25 +7008,28 @@
       </c>
       <c r="C7" s="60"/>
       <c r="D7" s="60"/>
-      <c r="E7" s="59"/>
+      <c r="E7" s="128" t="s">
+        <v>376</v>
+      </c>
       <c r="F7" s="59"/>
       <c r="G7" s="59"/>
       <c r="H7" s="59"/>
       <c r="I7" s="59"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
       <c r="L7" s="59"/>
       <c r="M7" s="59"/>
       <c r="N7" s="59"/>
       <c r="O7" s="59"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
       <c r="R7" s="59"/>
       <c r="S7" s="59"/>
       <c r="T7" s="59"/>
       <c r="U7" s="59"/>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" s="59"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="58" t="s">
         <v>315</v>
       </c>
@@ -6963,25 +7038,28 @@
       </c>
       <c r="C8" s="60"/>
       <c r="D8" s="60"/>
-      <c r="E8" s="59"/>
+      <c r="E8" s="128" t="s">
+        <v>377</v>
+      </c>
       <c r="F8" s="59"/>
       <c r="G8" s="59"/>
       <c r="H8" s="59"/>
       <c r="I8" s="59"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
       <c r="L8" s="59"/>
       <c r="M8" s="59"/>
       <c r="N8" s="59"/>
       <c r="O8" s="59"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="60"/>
       <c r="R8" s="59"/>
       <c r="S8" s="59"/>
       <c r="T8" s="59"/>
       <c r="U8" s="59"/>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="V8" s="59"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="58" t="s">
         <v>316</v>
       </c>
@@ -6990,25 +7068,28 @@
       </c>
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
-      <c r="E9" s="59"/>
+      <c r="E9" s="128" t="s">
+        <v>378</v>
+      </c>
       <c r="F9" s="59"/>
       <c r="G9" s="59"/>
       <c r="H9" s="59"/>
       <c r="I9" s="59"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
       <c r="N9" s="59"/>
       <c r="O9" s="59"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="60"/>
       <c r="R9" s="59"/>
       <c r="S9" s="59"/>
       <c r="T9" s="59"/>
       <c r="U9" s="59"/>
-    </row>
-    <row r="10" spans="1:21" ht="15.75">
+      <c r="V9" s="59"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75">
       <c r="A10" s="54" t="s">
         <v>360</v>
       </c>
@@ -7021,25 +7102,28 @@
       <c r="D10" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="128" t="s">
+        <v>379</v>
+      </c>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
       <c r="I10" s="55"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="56"/>
       <c r="L10" s="55"/>
       <c r="M10" s="55"/>
       <c r="N10" s="55"/>
       <c r="O10" s="55"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="56"/>
       <c r="R10" s="55"/>
       <c r="S10" s="55"/>
       <c r="T10" s="55"/>
-      <c r="U10" s="57"/>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="U10" s="55"/>
+      <c r="V10" s="57"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="58" t="s">
         <v>313</v>
       </c>
@@ -7048,25 +7132,28 @@
       </c>
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
-      <c r="E11" s="59"/>
+      <c r="E11" s="128" t="s">
+        <v>380</v>
+      </c>
       <c r="F11" s="59"/>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
       <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
       <c r="L11" s="59"/>
       <c r="M11" s="59"/>
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="60"/>
       <c r="R11" s="59"/>
       <c r="S11" s="59"/>
       <c r="T11" s="59"/>
       <c r="U11" s="59"/>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11" s="59"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="58" t="s">
         <v>145</v>
       </c>
@@ -7075,25 +7162,28 @@
       </c>
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
-      <c r="E12" s="59"/>
+      <c r="E12" s="128" t="s">
+        <v>381</v>
+      </c>
       <c r="F12" s="59"/>
       <c r="G12" s="59"/>
       <c r="H12" s="59"/>
       <c r="I12" s="59"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
       <c r="L12" s="59"/>
       <c r="M12" s="59"/>
       <c r="N12" s="59"/>
       <c r="O12" s="59"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="60"/>
       <c r="R12" s="59"/>
       <c r="S12" s="59"/>
       <c r="T12" s="59"/>
       <c r="U12" s="59"/>
-    </row>
-    <row r="13" spans="1:21" ht="15.75">
+      <c r="V12" s="59"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.75">
       <c r="A13" s="54" t="s">
         <v>361</v>
       </c>
@@ -7106,25 +7196,28 @@
       <c r="D13" s="120" t="s">
         <v>227</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="128" t="s">
+        <v>382</v>
+      </c>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
       <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="56"/>
       <c r="L13" s="55"/>
       <c r="M13" s="55"/>
       <c r="N13" s="55"/>
       <c r="O13" s="55"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="56"/>
       <c r="R13" s="55"/>
       <c r="S13" s="55"/>
       <c r="T13" s="55"/>
-      <c r="U13" s="57"/>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="U13" s="55"/>
+      <c r="V13" s="57"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="58" t="s">
         <v>362</v>
       </c>
@@ -7133,25 +7226,28 @@
       </c>
       <c r="C14" s="60"/>
       <c r="D14" s="60"/>
-      <c r="E14" s="59"/>
+      <c r="E14" s="128" t="s">
+        <v>383</v>
+      </c>
       <c r="F14" s="59"/>
       <c r="G14" s="59"/>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="60"/>
       <c r="L14" s="59"/>
       <c r="M14" s="59"/>
       <c r="N14" s="59"/>
       <c r="O14" s="59"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="59"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="60"/>
       <c r="R14" s="59"/>
       <c r="S14" s="59"/>
       <c r="T14" s="59"/>
       <c r="U14" s="59"/>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14" s="59"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="58" t="s">
         <v>363</v>
       </c>
@@ -7160,25 +7256,28 @@
       </c>
       <c r="C15" s="60"/>
       <c r="D15" s="60"/>
-      <c r="E15" s="59"/>
+      <c r="E15" s="128" t="s">
+        <v>384</v>
+      </c>
       <c r="F15" s="59"/>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
       <c r="L15" s="59"/>
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
       <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="60"/>
       <c r="R15" s="59"/>
       <c r="S15" s="59"/>
       <c r="T15" s="59"/>
       <c r="U15" s="59"/>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15" s="59"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="58" t="s">
         <v>364</v>
       </c>
@@ -7187,25 +7286,28 @@
       </c>
       <c r="C16" s="60"/>
       <c r="D16" s="60"/>
-      <c r="E16" s="59"/>
+      <c r="E16" s="128" t="s">
+        <v>385</v>
+      </c>
       <c r="F16" s="59"/>
       <c r="G16" s="59"/>
       <c r="H16" s="59"/>
       <c r="I16" s="59"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="60"/>
       <c r="L16" s="59"/>
       <c r="M16" s="59"/>
       <c r="N16" s="59"/>
       <c r="O16" s="59"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="60"/>
       <c r="R16" s="59"/>
       <c r="S16" s="59"/>
       <c r="T16" s="59"/>
       <c r="U16" s="59"/>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="V16" s="59"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="58" t="s">
         <v>365</v>
       </c>
@@ -7214,25 +7316,28 @@
       </c>
       <c r="C17" s="60"/>
       <c r="D17" s="60"/>
-      <c r="E17" s="59"/>
+      <c r="E17" s="128" t="s">
+        <v>386</v>
+      </c>
       <c r="F17" s="59"/>
       <c r="G17" s="59"/>
       <c r="H17" s="59"/>
       <c r="I17" s="59"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="60"/>
       <c r="L17" s="59"/>
       <c r="M17" s="59"/>
       <c r="N17" s="59"/>
       <c r="O17" s="59"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="60"/>
       <c r="R17" s="59"/>
       <c r="S17" s="59"/>
       <c r="T17" s="59"/>
       <c r="U17" s="59"/>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="V17" s="59"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="58" t="s">
         <v>366</v>
       </c>
@@ -7241,25 +7346,28 @@
       </c>
       <c r="C18" s="60"/>
       <c r="D18" s="60"/>
-      <c r="E18" s="59"/>
+      <c r="E18" s="128" t="s">
+        <v>387</v>
+      </c>
       <c r="F18" s="59"/>
       <c r="G18" s="59"/>
       <c r="H18" s="59"/>
       <c r="I18" s="59"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="60"/>
       <c r="L18" s="59"/>
       <c r="M18" s="59"/>
       <c r="N18" s="59"/>
       <c r="O18" s="59"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="60"/>
       <c r="R18" s="59"/>
       <c r="S18" s="59"/>
       <c r="T18" s="59"/>
       <c r="U18" s="59"/>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="V18" s="59"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="58" t="s">
         <v>145</v>
       </c>
@@ -7268,37 +7376,40 @@
       </c>
       <c r="C19" s="60"/>
       <c r="D19" s="60"/>
-      <c r="E19" s="59"/>
+      <c r="E19" s="128" t="s">
+        <v>388</v>
+      </c>
       <c r="F19" s="59"/>
       <c r="G19" s="59"/>
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="60"/>
       <c r="L19" s="59"/>
       <c r="M19" s="59"/>
       <c r="N19" s="59"/>
       <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="60"/>
       <c r="R19" s="59"/>
       <c r="S19" s="59"/>
       <c r="T19" s="59"/>
       <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="F3:J3"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q6:U9 E7:I9 K6:O9 Q11:T12 K11:O12 E11:I12 B5:B19">
+  <conditionalFormatting sqref="R6:V9 F7:J9 L6:P9 R11:U12 L11:P12 F11:J12 B5:B19">
     <cfRule type="cellIs" dxfId="83" priority="345" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7312,7 +7423,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U6">
+  <conditionalFormatting sqref="V6">
     <cfRule type="cellIs" dxfId="79" priority="353" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7326,7 +7437,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:I6">
+  <conditionalFormatting sqref="F6:J6">
     <cfRule type="cellIs" dxfId="75" priority="333" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7340,7 +7451,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U16:U19">
+  <conditionalFormatting sqref="V16:V19">
     <cfRule type="cellIs" dxfId="71" priority="141" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7354,7 +7465,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U14">
+  <conditionalFormatting sqref="V14">
     <cfRule type="cellIs" dxfId="67" priority="153" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7368,7 +7479,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:I14">
+  <conditionalFormatting sqref="F14:J14">
     <cfRule type="cellIs" dxfId="63" priority="149" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7382,7 +7493,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U15">
+  <conditionalFormatting sqref="V15">
     <cfRule type="cellIs" dxfId="59" priority="145" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7396,7 +7507,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:I19">
+  <conditionalFormatting sqref="F15:J19">
     <cfRule type="cellIs" dxfId="55" priority="137" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7410,7 +7521,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14:O19">
+  <conditionalFormatting sqref="L14:P19">
     <cfRule type="cellIs" dxfId="51" priority="133" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7424,7 +7535,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q14:T19">
+  <conditionalFormatting sqref="R14:U19">
     <cfRule type="cellIs" dxfId="47" priority="129" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7438,7 +7549,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U11:U12">
+  <conditionalFormatting sqref="V11:V12">
     <cfRule type="cellIs" dxfId="43" priority="113" operator="equal">
       <formula>"P"</formula>
     </cfRule>
@@ -7494,7 +7605,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B19" xr:uid="{B3D63F45-6CD8-4A3B-A6CE-99A81B46FAB0}">
       <formula1>types_unit_phase_descr</formula1>
     </dataValidation>
@@ -7594,7 +7705,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="133">
+      <c r="A4" s="135">
         <f>COUNTA(A6:A296)</f>
         <v>10</v>
       </c>
@@ -7620,7 +7731,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="133"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="108"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -12169,8 +12280,8 @@
   </sheetPr>
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12191,18 +12302,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="146" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="E2" s="144" t="s">
+      <c r="C2" s="147"/>
+      <c r="E2" s="146" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="145"/>
-      <c r="H2" s="144" t="s">
+      <c r="F2" s="147"/>
+      <c r="H2" s="146" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="145"/>
+      <c r="I2" s="147"/>
       <c r="K2" s="116" t="s">
         <v>359</v>
       </c>
@@ -12433,11 +12544,11 @@
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="M1" s="134" t="str">
+      <c r="M1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="135"/>
+      <c r="N1" s="137"/>
     </row>
     <row r="2" spans="1:999" ht="18" customHeight="1">
       <c r="A2" s="42"/>
@@ -12455,11 +12566,11 @@
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="M2" s="134" t="str">
+      <c r="M2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="135"/>
+      <c r="N2" s="137"/>
     </row>
     <row r="3" spans="1:999" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -12510,7 +12621,7 @@
     </row>
     <row r="4" spans="1:999" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B293)</f>
         <v>57</v>
       </c>
@@ -12553,7 +12664,7 @@
     </row>
     <row r="5" spans="1:999" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -18792,7 +18903,7 @@
     </row>
     <row r="4" spans="1:1009" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B300)</f>
         <v>14</v>
       </c>
@@ -18825,7 +18936,7 @@
     </row>
     <row r="5" spans="1:1009" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -24198,7 +24309,7 @@
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B303)</f>
         <v>17</v>
       </c>
@@ -24224,7 +24335,7 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -27828,7 +27939,7 @@
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B300)</f>
         <v>1</v>
       </c>
@@ -27858,7 +27969,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -31544,16 +31655,16 @@
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
       <c r="I1" s="43"/>
-      <c r="J1" s="136" t="str">
+      <c r="J1" s="138" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="K1" s="136"/>
-      <c r="L1" s="134" t="str">
+      <c r="K1" s="138"/>
+      <c r="L1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="135"/>
+      <c r="M1" s="137"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="43"/>
@@ -31565,16 +31676,16 @@
       <c r="G2" s="43"/>
       <c r="H2" s="43"/>
       <c r="I2" s="43"/>
-      <c r="J2" s="136" t="str">
+      <c r="J2" s="138" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134" t="str">
+      <c r="K2" s="138"/>
+      <c r="L2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="135"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -31619,7 +31730,7 @@
     </row>
     <row r="4" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B300)</f>
         <v>18</v>
       </c>
@@ -31652,7 +31763,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -36553,16 +36664,16 @@
       <c r="F1" s="39"/>
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
-      <c r="I1" s="136" t="str">
+      <c r="I1" s="138" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="J1" s="136"/>
-      <c r="K1" s="134" t="str">
+      <c r="J1" s="138"/>
+      <c r="K1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="L1" s="135"/>
+      <c r="L1" s="137"/>
     </row>
     <row r="2" spans="1:1019" ht="18" customHeight="1">
       <c r="A2" s="22"/>
@@ -36573,16 +36684,16 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
-      <c r="I2" s="136" t="str">
+      <c r="I2" s="138" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="J2" s="136"/>
-      <c r="K2" s="134" t="str">
+      <c r="J2" s="138"/>
+      <c r="K2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="L2" s="135"/>
+      <c r="L2" s="137"/>
     </row>
     <row r="3" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -36625,7 +36736,7 @@
     </row>
     <row r="4" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B300)</f>
         <v>42</v>
       </c>
@@ -36655,7 +36766,7 @@
     </row>
     <row r="5" spans="1:1019" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -41431,16 +41542,16 @@
       <c r="H1" s="43"/>
       <c r="I1" s="43"/>
       <c r="J1" s="43"/>
-      <c r="K1" s="136" t="str">
+      <c r="K1" s="138" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="L1" s="136"/>
-      <c r="M1" s="134" t="str">
+      <c r="L1" s="138"/>
+      <c r="M1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="135"/>
+      <c r="N1" s="137"/>
       <c r="O1" s="43"/>
       <c r="P1" s="43"/>
     </row>
@@ -41455,16 +41566,16 @@
       <c r="H2" s="43"/>
       <c r="I2" s="43"/>
       <c r="J2" s="43"/>
-      <c r="K2" s="136" t="str">
+      <c r="K2" s="138" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="L2" s="136"/>
-      <c r="M2" s="134" t="str">
+      <c r="L2" s="138"/>
+      <c r="M2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="135"/>
+      <c r="N2" s="137"/>
       <c r="O2" s="43"/>
       <c r="P2" s="43"/>
     </row>
@@ -41508,15 +41619,15 @@
       <c r="M3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="137" t="s">
+      <c r="N3" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="137"/>
-      <c r="P3" s="137"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
     </row>
     <row r="4" spans="1:16" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B299)</f>
         <v>12</v>
       </c>
@@ -41552,7 +41663,7 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -47113,16 +47224,16 @@
       <c r="G1" s="43"/>
       <c r="H1" s="43"/>
       <c r="I1" s="43"/>
-      <c r="J1" s="136" t="str">
+      <c r="J1" s="138" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="K1" s="136"/>
-      <c r="L1" s="134" t="str">
+      <c r="K1" s="138"/>
+      <c r="L1" s="136" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="135"/>
+      <c r="M1" s="137"/>
     </row>
     <row r="2" spans="1:13" s="24" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="43"/>
@@ -47134,16 +47245,16 @@
       <c r="G2" s="43"/>
       <c r="H2" s="43"/>
       <c r="I2" s="43"/>
-      <c r="J2" s="136" t="str">
+      <c r="J2" s="138" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="K2" s="136"/>
-      <c r="L2" s="134" t="str">
+      <c r="K2" s="138"/>
+      <c r="L2" s="136" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="135"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="40" t="s">
@@ -47188,7 +47299,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="133">
+      <c r="B4" s="135">
         <f>COUNTA(B6:B300)</f>
         <v>7</v>
       </c>
@@ -47218,7 +47329,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="133"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>

</xml_diff>

<commit_message>
cleanup and create exe
</commit_message>
<xml_diff>
--- a/latest_td.xlsx
+++ b/latest_td.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://martenssonconsultingse-my.sharepoint.com/personal/gustav_martenssonconsulting_se/Documents/10 Github Project/automation-boilerplate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EddieKarlsson\Project\github\automation-boilerplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B2740E02-08BC-47F5-AF20-77E934150726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD18F9A7-1D3B-4A7E-89DE-2DDB2A3305FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25C9723-2161-420A-98C5-EF94ACEE1DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA7251AA-4BA0-402A-BD93-E22E271F770A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2334,43 +2334,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -2476,6 +2439,37 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2685,24 +2679,67 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="19" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="20" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="6" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="16" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="44" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="17" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="40" fillId="6" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="16" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="33" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2711,15 +2748,6 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="7" borderId="35" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2742,16 +2770,16 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="16" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="17" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="17" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="18" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="16" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2760,55 +2788,24 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="46" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="19" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="20" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="6" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="16" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="9" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="47" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="17" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="40" fillId="6" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="16" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6097,7 +6094,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6396,8 +6393,8 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:AMC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6657,62 +6654,62 @@
       <c r="F12" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A31" s="87" t="s">
+      <c r="A31" s="104" t="s">
         <v>327</v>
       </c>
-      <c r="B31" s="88"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="89"/>
-    </row>
-    <row r="32" spans="1:6" ht="97.5" customHeight="1" thickBot="1">
+      <c r="B31" s="105"/>
+      <c r="C31" s="105"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="106"/>
+    </row>
+    <row r="32" spans="1:6" ht="97.5" customHeight="1">
       <c r="A32" s="69" t="s">
         <v>324</v>
       </c>
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="120" t="s">
         <v>356</v>
       </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="92"/>
-    </row>
-    <row r="33" spans="1:6" ht="32.25" customHeight="1" thickBot="1">
+      <c r="C32" s="121"/>
+      <c r="D32" s="121"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="122"/>
+    </row>
+    <row r="33" spans="1:6" ht="32.25" customHeight="1">
       <c r="A33" s="69" t="s">
         <v>372</v>
       </c>
-      <c r="B33" s="90" t="s">
+      <c r="B33" s="123" t="s">
         <v>373</v>
       </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="92"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="124"/>
+      <c r="F33" s="125"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="69" t="s">
         <v>392</v>
       </c>
-      <c r="B34" s="90" t="s">
+      <c r="B34" s="123" t="s">
         <v>393</v>
       </c>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="92"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="125"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="69" t="s">
         <v>405</v>
       </c>
-      <c r="B35" s="90" t="s">
+      <c r="B35" s="123" t="s">
         <v>406</v>
       </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="92"/>
+      <c r="C35" s="124"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="125"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:A12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -6785,7 +6782,7 @@
   <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6793,7 +6790,7 @@
     <col min="1" max="1" width="28.140625" style="40" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" style="40" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="40" hidden="1" customWidth="1"/>
     <col min="6" max="10" width="10.7109375" style="40" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" style="40" customWidth="1"/>
     <col min="12" max="16" width="10.7109375" style="40" customWidth="1"/>
@@ -6804,1256 +6801,1256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18" customHeight="1" thickBot="1">
-      <c r="A1" s="117"/>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="96" t="s">
+      <c r="A1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="110" t="s">
         <v>310</v>
       </c>
-      <c r="T1" s="96"/>
-      <c r="U1" s="94" t="s">
+      <c r="T1" s="110"/>
+      <c r="U1" s="108" t="s">
         <v>311</v>
       </c>
-      <c r="V1" s="95"/>
+      <c r="V1" s="109"/>
     </row>
     <row r="2" spans="1:22" ht="18" customHeight="1">
-      <c r="A2" s="117"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="96" t="s">
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="110" t="s">
         <v>309</v>
       </c>
-      <c r="T2" s="96"/>
-      <c r="U2" s="94" t="s">
+      <c r="T2" s="110"/>
+      <c r="U2" s="108" t="s">
         <v>312</v>
       </c>
-      <c r="V2" s="95"/>
+      <c r="V2" s="109"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="112" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="98" t="s">
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="112" t="s">
         <v>196</v>
       </c>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="98" t="s">
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="112" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="99" t="s">
+      <c r="M3" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="N3" s="99" t="s">
+      <c r="N3" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="O3" s="99" t="s">
+      <c r="O3" s="113" t="s">
         <v>197</v>
       </c>
-      <c r="P3" s="100" t="s">
+      <c r="P3" s="117" t="s">
         <v>197</v>
       </c>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="98" t="s">
+      <c r="Q3" s="96"/>
+      <c r="R3" s="112" t="s">
         <v>198</v>
       </c>
-      <c r="S3" s="99" t="s">
+      <c r="S3" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="T3" s="99" t="s">
+      <c r="T3" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="99" t="s">
+      <c r="U3" s="113" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="102" t="s">
+      <c r="V3" s="114" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="41" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="97" t="s">
         <v>358</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="97" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="119" t="s">
+      <c r="E4" s="97" t="s">
         <v>389</v>
       </c>
-      <c r="F4" s="120" t="s">
+      <c r="F4" s="98" t="s">
         <v>199</v>
       </c>
-      <c r="G4" s="120" t="s">
+      <c r="G4" s="98" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="120" t="s">
+      <c r="H4" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="I4" s="120" t="s">
+      <c r="I4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="120" t="s">
+      <c r="J4" s="98" t="s">
         <v>202</v>
       </c>
-      <c r="K4" s="121"/>
-      <c r="L4" s="120" t="s">
+      <c r="K4" s="99"/>
+      <c r="L4" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="M4" s="120" t="s">
+      <c r="M4" s="98" t="s">
         <v>204</v>
       </c>
-      <c r="N4" s="120" t="s">
+      <c r="N4" s="98" t="s">
         <v>205</v>
       </c>
-      <c r="O4" s="120" t="s">
+      <c r="O4" s="98" t="s">
         <v>206</v>
       </c>
-      <c r="P4" s="120" t="s">
+      <c r="P4" s="98" t="s">
         <v>207</v>
       </c>
-      <c r="Q4" s="121"/>
-      <c r="R4" s="120" t="s">
+      <c r="Q4" s="99"/>
+      <c r="R4" s="98" t="s">
         <v>208</v>
       </c>
-      <c r="S4" s="120" t="s">
+      <c r="S4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="120" t="s">
+      <c r="T4" s="98" t="s">
         <v>209</v>
       </c>
-      <c r="U4" s="120" t="s">
+      <c r="U4" s="98" t="s">
         <v>210</v>
       </c>
-      <c r="V4" s="103"/>
+      <c r="V4" s="115"/>
     </row>
     <row r="5" spans="1:22" ht="15.75">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="90" t="s">
         <v>357</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="122" t="s">
+      <c r="D5" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="114"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="93"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="124" t="s">
+      <c r="A6" s="102" t="s">
         <v>314</v>
       </c>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="123" t="s">
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="94"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="123" t="s">
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
-      <c r="H7" s="115"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="115"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="115"/>
-      <c r="O7" s="115"/>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="115"/>
-      <c r="S7" s="115"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="94"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="94"/>
+      <c r="V7" s="94"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="123" t="s">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="101" t="s">
         <v>377</v>
       </c>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="115"/>
-      <c r="K8" s="125"/>
-      <c r="L8" s="115"/>
-      <c r="M8" s="115"/>
-      <c r="N8" s="115"/>
-      <c r="O8" s="115"/>
-      <c r="P8" s="115"/>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="115"/>
-      <c r="S8" s="115"/>
-      <c r="T8" s="115"/>
-      <c r="U8" s="115"/>
-      <c r="V8" s="115"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="94"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="94"/>
+      <c r="V8" s="94"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="102" t="s">
         <v>316</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="123" t="s">
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="101" t="s">
         <v>378</v>
       </c>
-      <c r="F9" s="115"/>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="115"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="115"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="115"/>
-      <c r="O9" s="115"/>
-      <c r="P9" s="115"/>
-      <c r="Q9" s="125"/>
-      <c r="R9" s="115"/>
-      <c r="S9" s="115"/>
-      <c r="T9" s="115"/>
-      <c r="U9" s="115"/>
-      <c r="V9" s="115"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="94"/>
+      <c r="S9" s="94"/>
+      <c r="T9" s="94"/>
+      <c r="U9" s="94"/>
+      <c r="V9" s="94"/>
     </row>
     <row r="10" spans="1:22" ht="15.75">
-      <c r="A10" s="111" t="s">
+      <c r="A10" s="90" t="s">
         <v>396</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="123" t="s">
+      <c r="E10" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="112"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="112"/>
-      <c r="N10" s="112"/>
-      <c r="O10" s="112"/>
-      <c r="P10" s="112"/>
-      <c r="Q10" s="113"/>
-      <c r="R10" s="112"/>
-      <c r="S10" s="112"/>
-      <c r="T10" s="112"/>
-      <c r="U10" s="112"/>
-      <c r="V10" s="114"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="91"/>
+      <c r="Q10" s="92"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="93"/>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="102" t="s">
         <v>314</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="123" t="s">
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="F11" s="115"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="125"/>
-      <c r="L11" s="115"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="115"/>
-      <c r="P11" s="115"/>
-      <c r="Q11" s="125"/>
-      <c r="R11" s="115"/>
-      <c r="S11" s="115"/>
-      <c r="T11" s="115"/>
-      <c r="U11" s="115"/>
-      <c r="V11" s="115"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="94"/>
+      <c r="O11" s="94"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="94"/>
+      <c r="S11" s="94"/>
+      <c r="T11" s="94"/>
+      <c r="U11" s="94"/>
+      <c r="V11" s="94"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="123" t="s">
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="F12" s="115"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="125"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="115"/>
-      <c r="N12" s="115"/>
-      <c r="O12" s="115"/>
-      <c r="P12" s="115"/>
-      <c r="Q12" s="125"/>
-      <c r="R12" s="115"/>
-      <c r="S12" s="115"/>
-      <c r="T12" s="115"/>
-      <c r="U12" s="115"/>
-      <c r="V12" s="115"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="103"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="94"/>
+      <c r="O12" s="94"/>
+      <c r="P12" s="94"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="94"/>
+      <c r="S12" s="94"/>
+      <c r="T12" s="94"/>
+      <c r="U12" s="94"/>
+      <c r="V12" s="94"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="123" t="s">
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="101" t="s">
         <v>377</v>
       </c>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="115"/>
-      <c r="N13" s="115"/>
-      <c r="O13" s="115"/>
-      <c r="P13" s="115"/>
-      <c r="Q13" s="125"/>
-      <c r="R13" s="115"/>
-      <c r="S13" s="115"/>
-      <c r="T13" s="115"/>
-      <c r="U13" s="115"/>
-      <c r="V13" s="115"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="94"/>
+      <c r="S13" s="94"/>
+      <c r="T13" s="94"/>
+      <c r="U13" s="94"/>
+      <c r="V13" s="94"/>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="102" t="s">
         <v>316</v>
       </c>
-      <c r="B14" s="122" t="s">
+      <c r="B14" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="123" t="s">
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="101" t="s">
         <v>378</v>
       </c>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="115"/>
-      <c r="I14" s="115"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="125"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
-      <c r="N14" s="115"/>
-      <c r="O14" s="115"/>
-      <c r="P14" s="115"/>
-      <c r="Q14" s="125"/>
-      <c r="R14" s="115"/>
-      <c r="S14" s="115"/>
-      <c r="T14" s="115"/>
-      <c r="U14" s="115"/>
-      <c r="V14" s="115"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="103"/>
+      <c r="L14" s="94"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="94"/>
+      <c r="S14" s="94"/>
+      <c r="T14" s="94"/>
+      <c r="U14" s="94"/>
+      <c r="V14" s="94"/>
     </row>
     <row r="15" spans="1:22" ht="15.75">
-      <c r="A15" s="111" t="s">
+      <c r="A15" s="90" t="s">
         <v>360</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="123" t="s">
+      <c r="E15" s="101" t="s">
         <v>379</v>
       </c>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="112"/>
-      <c r="P15" s="112"/>
-      <c r="Q15" s="113"/>
-      <c r="R15" s="112"/>
-      <c r="S15" s="112"/>
-      <c r="T15" s="112"/>
-      <c r="U15" s="112"/>
-      <c r="V15" s="114"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="93"/>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="123" t="s">
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="101" t="s">
         <v>380</v>
       </c>
-      <c r="F16" s="115"/>
-      <c r="G16" s="115"/>
-      <c r="H16" s="115"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="125"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
-      <c r="N16" s="115"/>
-      <c r="O16" s="115"/>
-      <c r="P16" s="115"/>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="115"/>
-      <c r="S16" s="115"/>
-      <c r="T16" s="115"/>
-      <c r="U16" s="115"/>
-      <c r="V16" s="115"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="94"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="94"/>
+      <c r="T16" s="94"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="123" t="s">
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="125"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="115"/>
-      <c r="O17" s="115"/>
-      <c r="P17" s="115"/>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="115"/>
-      <c r="S17" s="115"/>
-      <c r="T17" s="115"/>
-      <c r="U17" s="115"/>
-      <c r="V17" s="115"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="94"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="103"/>
+      <c r="R17" s="94"/>
+      <c r="S17" s="94"/>
+      <c r="T17" s="94"/>
+      <c r="U17" s="94"/>
+      <c r="V17" s="94"/>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="124" t="s">
+      <c r="A18" s="102" t="s">
         <v>357</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="100" t="s">
         <v>394</v>
       </c>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="123" t="s">
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F18" s="115"/>
-      <c r="G18" s="115"/>
-      <c r="H18" s="115"/>
-      <c r="I18" s="115"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="115"/>
-      <c r="N18" s="115"/>
-      <c r="O18" s="115"/>
-      <c r="P18" s="115"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="115"/>
-      <c r="S18" s="115"/>
-      <c r="T18" s="115"/>
-      <c r="U18" s="115"/>
-      <c r="V18" s="115"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="94"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="94"/>
+      <c r="S18" s="94"/>
+      <c r="T18" s="94"/>
+      <c r="U18" s="94"/>
+      <c r="V18" s="94"/>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="102" t="s">
         <v>396</v>
       </c>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="100" t="s">
         <v>394</v>
       </c>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="123" t="s">
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F19" s="115"/>
-      <c r="G19" s="115"/>
-      <c r="H19" s="115"/>
-      <c r="I19" s="115"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
-      <c r="N19" s="115"/>
-      <c r="O19" s="115"/>
-      <c r="P19" s="115"/>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="115"/>
-      <c r="S19" s="115"/>
-      <c r="T19" s="115"/>
-      <c r="U19" s="115"/>
-      <c r="V19" s="115"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="103"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="94"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="94"/>
+      <c r="Q19" s="103"/>
+      <c r="R19" s="94"/>
+      <c r="S19" s="94"/>
+      <c r="T19" s="94"/>
+      <c r="U19" s="94"/>
+      <c r="V19" s="94"/>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="124" t="s">
+      <c r="A20" s="102" t="s">
         <v>361</v>
       </c>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="100" t="s">
         <v>395</v>
       </c>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="123" t="s">
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F20" s="115"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="115"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="125"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
-      <c r="N20" s="115"/>
-      <c r="O20" s="115"/>
-      <c r="P20" s="115"/>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="115"/>
-      <c r="S20" s="115"/>
-      <c r="T20" s="115"/>
-      <c r="U20" s="115"/>
-      <c r="V20" s="115"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="94"/>
+      <c r="O20" s="94"/>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="94"/>
+      <c r="S20" s="94"/>
+      <c r="T20" s="94"/>
+      <c r="U20" s="94"/>
+      <c r="V20" s="94"/>
     </row>
     <row r="21" spans="1:22" ht="15.75">
-      <c r="A21" s="111" t="s">
+      <c r="A21" s="90" t="s">
         <v>361</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="100" t="s">
         <v>227</v>
       </c>
-      <c r="E21" s="123" t="s">
+      <c r="E21" s="101" t="s">
         <v>382</v>
       </c>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="112"/>
-      <c r="M21" s="112"/>
-      <c r="N21" s="112"/>
-      <c r="O21" s="112"/>
-      <c r="P21" s="112"/>
-      <c r="Q21" s="113"/>
-      <c r="R21" s="112"/>
-      <c r="S21" s="112"/>
-      <c r="T21" s="112"/>
-      <c r="U21" s="112"/>
-      <c r="V21" s="114"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="91"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="92"/>
+      <c r="R21" s="91"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="91"/>
+      <c r="U21" s="91"/>
+      <c r="V21" s="93"/>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="124" t="s">
+      <c r="A22" s="102" t="s">
         <v>362</v>
       </c>
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="123" t="s">
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="115"/>
-      <c r="K22" s="125"/>
-      <c r="L22" s="115"/>
-      <c r="M22" s="115"/>
-      <c r="N22" s="115"/>
-      <c r="O22" s="115"/>
-      <c r="P22" s="115"/>
-      <c r="Q22" s="125"/>
-      <c r="R22" s="115"/>
-      <c r="S22" s="115"/>
-      <c r="T22" s="115"/>
-      <c r="U22" s="115"/>
-      <c r="V22" s="115"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="103"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="94"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="103"/>
+      <c r="R22" s="94"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="94"/>
+      <c r="U22" s="94"/>
+      <c r="V22" s="94"/>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="102" t="s">
         <v>363</v>
       </c>
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="123" t="s">
+      <c r="C23" s="103"/>
+      <c r="D23" s="103"/>
+      <c r="E23" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="F23" s="115"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="115"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="115"/>
-      <c r="K23" s="125"/>
-      <c r="L23" s="115"/>
-      <c r="M23" s="115"/>
-      <c r="N23" s="115"/>
-      <c r="O23" s="115"/>
-      <c r="P23" s="115"/>
-      <c r="Q23" s="125"/>
-      <c r="R23" s="115"/>
-      <c r="S23" s="115"/>
-      <c r="T23" s="115"/>
-      <c r="U23" s="115"/>
-      <c r="V23" s="115"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="103"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="94"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="94"/>
+      <c r="Q23" s="103"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="94"/>
+      <c r="T23" s="94"/>
+      <c r="U23" s="94"/>
+      <c r="V23" s="94"/>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="102" t="s">
         <v>364</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="125"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="123" t="s">
+      <c r="C24" s="103"/>
+      <c r="D24" s="103"/>
+      <c r="E24" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="F24" s="115"/>
-      <c r="G24" s="115"/>
-      <c r="H24" s="115"/>
-      <c r="I24" s="115"/>
-      <c r="J24" s="115"/>
-      <c r="K24" s="125"/>
-      <c r="L24" s="115"/>
-      <c r="M24" s="115"/>
-      <c r="N24" s="115"/>
-      <c r="O24" s="115"/>
-      <c r="P24" s="115"/>
-      <c r="Q24" s="125"/>
-      <c r="R24" s="115"/>
-      <c r="S24" s="115"/>
-      <c r="T24" s="115"/>
-      <c r="U24" s="115"/>
-      <c r="V24" s="115"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="103"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="94"/>
+      <c r="N24" s="94"/>
+      <c r="O24" s="94"/>
+      <c r="P24" s="94"/>
+      <c r="Q24" s="103"/>
+      <c r="R24" s="94"/>
+      <c r="S24" s="94"/>
+      <c r="T24" s="94"/>
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="102" t="s">
         <v>365</v>
       </c>
-      <c r="B25" s="122" t="s">
+      <c r="B25" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="123" t="s">
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
+      <c r="E25" s="101" t="s">
         <v>386</v>
       </c>
-      <c r="F25" s="115"/>
-      <c r="G25" s="115"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="115"/>
-      <c r="K25" s="125"/>
-      <c r="L25" s="115"/>
-      <c r="M25" s="115"/>
-      <c r="N25" s="115"/>
-      <c r="O25" s="115"/>
-      <c r="P25" s="115"/>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="115"/>
-      <c r="S25" s="115"/>
-      <c r="T25" s="115"/>
-      <c r="U25" s="115"/>
-      <c r="V25" s="115"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="103"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="94"/>
+      <c r="O25" s="94"/>
+      <c r="P25" s="94"/>
+      <c r="Q25" s="103"/>
+      <c r="R25" s="94"/>
+      <c r="S25" s="94"/>
+      <c r="T25" s="94"/>
+      <c r="U25" s="94"/>
+      <c r="V25" s="94"/>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" s="124" t="s">
+      <c r="A26" s="102" t="s">
         <v>366</v>
       </c>
-      <c r="B26" s="122" t="s">
+      <c r="B26" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="123" t="s">
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="101" t="s">
         <v>387</v>
       </c>
-      <c r="F26" s="115"/>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="115"/>
-      <c r="J26" s="115"/>
-      <c r="K26" s="125"/>
-      <c r="L26" s="115"/>
-      <c r="M26" s="115"/>
-      <c r="N26" s="115"/>
-      <c r="O26" s="115"/>
-      <c r="P26" s="115"/>
-      <c r="Q26" s="125"/>
-      <c r="R26" s="115"/>
-      <c r="S26" s="115"/>
-      <c r="T26" s="115"/>
-      <c r="U26" s="115"/>
-      <c r="V26" s="115"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="94"/>
+      <c r="I26" s="94"/>
+      <c r="J26" s="94"/>
+      <c r="K26" s="103"/>
+      <c r="L26" s="94"/>
+      <c r="M26" s="94"/>
+      <c r="N26" s="94"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="103"/>
+      <c r="R26" s="94"/>
+      <c r="S26" s="94"/>
+      <c r="T26" s="94"/>
+      <c r="U26" s="94"/>
+      <c r="V26" s="94"/>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="124" t="s">
+      <c r="A27" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="123" t="s">
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="101" t="s">
         <v>388</v>
       </c>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="125"/>
-      <c r="L27" s="115"/>
-      <c r="M27" s="115"/>
-      <c r="N27" s="115"/>
-      <c r="O27" s="115"/>
-      <c r="P27" s="115"/>
-      <c r="Q27" s="125"/>
-      <c r="R27" s="115"/>
-      <c r="S27" s="115"/>
-      <c r="T27" s="115"/>
-      <c r="U27" s="115"/>
-      <c r="V27" s="115"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="94"/>
+      <c r="M27" s="94"/>
+      <c r="N27" s="94"/>
+      <c r="O27" s="94"/>
+      <c r="P27" s="94"/>
+      <c r="Q27" s="103"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="94"/>
+      <c r="T27" s="94"/>
+      <c r="U27" s="94"/>
+      <c r="V27" s="94"/>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="124" t="s">
+      <c r="A28" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="B28" s="122" t="s">
+      <c r="B28" s="100" t="s">
         <v>395</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="123" t="s">
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="115"/>
-      <c r="M28" s="115"/>
-      <c r="N28" s="115"/>
-      <c r="O28" s="115"/>
-      <c r="P28" s="115"/>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="115"/>
-      <c r="S28" s="115"/>
-      <c r="T28" s="115"/>
-      <c r="U28" s="115"/>
-      <c r="V28" s="115"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="103"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
+      <c r="N28" s="94"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="103"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="94"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="94"/>
+      <c r="V28" s="94"/>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="124" t="s">
+      <c r="A29" s="102" t="s">
         <v>398</v>
       </c>
-      <c r="B29" s="122" t="s">
+      <c r="B29" s="100" t="s">
         <v>395</v>
       </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="123" t="s">
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="101" t="s">
         <v>381</v>
       </c>
-      <c r="F29" s="115"/>
-      <c r="G29" s="115"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="115"/>
-      <c r="J29" s="115"/>
-      <c r="K29" s="125"/>
-      <c r="L29" s="115"/>
-      <c r="M29" s="115"/>
-      <c r="N29" s="115"/>
-      <c r="O29" s="115"/>
-      <c r="P29" s="115"/>
-      <c r="Q29" s="125"/>
-      <c r="R29" s="115"/>
-      <c r="S29" s="115"/>
-      <c r="T29" s="115"/>
-      <c r="U29" s="115"/>
-      <c r="V29" s="115"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
     </row>
     <row r="30" spans="1:22" ht="15.75">
-      <c r="A30" s="111" t="s">
+      <c r="A30" s="90" t="s">
         <v>397</v>
       </c>
-      <c r="B30" s="122" t="s">
+      <c r="B30" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="122" t="s">
+      <c r="D30" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="123" t="s">
+      <c r="E30" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="113"/>
-      <c r="L30" s="112"/>
-      <c r="M30" s="112"/>
-      <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
-      <c r="P30" s="112"/>
-      <c r="Q30" s="113"/>
-      <c r="R30" s="112"/>
-      <c r="S30" s="112"/>
-      <c r="T30" s="112"/>
-      <c r="U30" s="112"/>
-      <c r="V30" s="114"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="92"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="93"/>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="124" t="s">
+      <c r="A31" s="102" t="s">
         <v>314</v>
       </c>
-      <c r="B31" s="122" t="s">
+      <c r="B31" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="123" t="s">
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="115"/>
-      <c r="I31" s="115"/>
-      <c r="J31" s="115"/>
-      <c r="K31" s="125"/>
-      <c r="L31" s="115"/>
-      <c r="M31" s="115"/>
-      <c r="N31" s="115"/>
-      <c r="O31" s="115"/>
-      <c r="P31" s="115"/>
-      <c r="Q31" s="125"/>
-      <c r="R31" s="115"/>
-      <c r="S31" s="115"/>
-      <c r="T31" s="115"/>
-      <c r="U31" s="115"/>
-      <c r="V31" s="115"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="103"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="124" t="s">
+      <c r="A32" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="122" t="s">
+      <c r="B32" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="123" t="s">
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="125"/>
-      <c r="L32" s="115"/>
-      <c r="M32" s="115"/>
-      <c r="N32" s="115"/>
-      <c r="O32" s="115"/>
-      <c r="P32" s="115"/>
-      <c r="Q32" s="125"/>
-      <c r="R32" s="115"/>
-      <c r="S32" s="115"/>
-      <c r="T32" s="115"/>
-      <c r="U32" s="115"/>
-      <c r="V32" s="115"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
+      <c r="V32" s="94"/>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="124" t="s">
+      <c r="A33" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="B33" s="122" t="s">
+      <c r="B33" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C33" s="125"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="123" t="s">
+      <c r="C33" s="103"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="101" t="s">
         <v>377</v>
       </c>
-      <c r="F33" s="115"/>
-      <c r="G33" s="115"/>
-      <c r="H33" s="115"/>
-      <c r="I33" s="115"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="125"/>
-      <c r="L33" s="115"/>
-      <c r="M33" s="115"/>
-      <c r="N33" s="115"/>
-      <c r="O33" s="115"/>
-      <c r="P33" s="115"/>
-      <c r="Q33" s="125"/>
-      <c r="R33" s="115"/>
-      <c r="S33" s="115"/>
-      <c r="T33" s="115"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="103"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="103"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="124" t="s">
+      <c r="A34" s="102" t="s">
         <v>316</v>
       </c>
-      <c r="B34" s="122" t="s">
+      <c r="B34" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="123" t="s">
+      <c r="C34" s="103"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="101" t="s">
         <v>378</v>
       </c>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="125"/>
-      <c r="L34" s="115"/>
-      <c r="M34" s="115"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="115"/>
-      <c r="P34" s="115"/>
-      <c r="Q34" s="125"/>
-      <c r="R34" s="115"/>
-      <c r="S34" s="115"/>
-      <c r="T34" s="115"/>
-      <c r="U34" s="115"/>
-      <c r="V34" s="115"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="94"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="94"/>
+      <c r="K34" s="103"/>
+      <c r="L34" s="94"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="94"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="94"/>
+      <c r="Q34" s="103"/>
+      <c r="R34" s="94"/>
+      <c r="S34" s="94"/>
+      <c r="T34" s="94"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
     </row>
     <row r="35" spans="1:22" ht="15.75">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="90" t="s">
         <v>398</v>
       </c>
-      <c r="B35" s="122" t="s">
+      <c r="B35" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="122" t="s">
+      <c r="D35" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="123" t="s">
+      <c r="E35" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="112"/>
-      <c r="M35" s="112"/>
-      <c r="N35" s="112"/>
-      <c r="O35" s="112"/>
-      <c r="P35" s="112"/>
-      <c r="Q35" s="113"/>
-      <c r="R35" s="112"/>
-      <c r="S35" s="112"/>
-      <c r="T35" s="112"/>
-      <c r="U35" s="112"/>
-      <c r="V35" s="114"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="91"/>
+      <c r="J35" s="91"/>
+      <c r="K35" s="92"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="91"/>
+      <c r="Q35" s="92"/>
+      <c r="R35" s="91"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
+      <c r="V35" s="93"/>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="124" t="s">
+      <c r="A36" s="102" t="s">
         <v>314</v>
       </c>
-      <c r="B36" s="122" t="s">
+      <c r="B36" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="123" t="s">
+      <c r="C36" s="103"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="F36" s="115"/>
-      <c r="G36" s="115"/>
-      <c r="H36" s="115"/>
-      <c r="I36" s="115"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="125"/>
-      <c r="L36" s="115"/>
-      <c r="M36" s="115"/>
-      <c r="N36" s="115"/>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
-      <c r="Q36" s="125"/>
-      <c r="R36" s="115"/>
-      <c r="S36" s="115"/>
-      <c r="T36" s="115"/>
-      <c r="U36" s="115"/>
-      <c r="V36" s="115"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="94"/>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="103"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="94"/>
+      <c r="N36" s="94"/>
+      <c r="O36" s="94"/>
+      <c r="P36" s="94"/>
+      <c r="Q36" s="103"/>
+      <c r="R36" s="94"/>
+      <c r="S36" s="94"/>
+      <c r="T36" s="94"/>
+      <c r="U36" s="94"/>
+      <c r="V36" s="94"/>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="124" t="s">
+      <c r="A37" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="122" t="s">
+      <c r="B37" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C37" s="125"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="123" t="s">
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="F37" s="115"/>
-      <c r="G37" s="115"/>
-      <c r="H37" s="115"/>
-      <c r="I37" s="115"/>
-      <c r="J37" s="115"/>
-      <c r="K37" s="125"/>
-      <c r="L37" s="115"/>
-      <c r="M37" s="115"/>
-      <c r="N37" s="115"/>
-      <c r="O37" s="115"/>
-      <c r="P37" s="115"/>
-      <c r="Q37" s="125"/>
-      <c r="R37" s="115"/>
-      <c r="S37" s="115"/>
-      <c r="T37" s="115"/>
-      <c r="U37" s="115"/>
-      <c r="V37" s="115"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="103"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="94"/>
+      <c r="O37" s="94"/>
+      <c r="P37" s="94"/>
+      <c r="Q37" s="103"/>
+      <c r="R37" s="94"/>
+      <c r="S37" s="94"/>
+      <c r="T37" s="94"/>
+      <c r="U37" s="94"/>
+      <c r="V37" s="94"/>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="124" t="s">
+      <c r="A38" s="102" t="s">
         <v>315</v>
       </c>
-      <c r="B38" s="122" t="s">
+      <c r="B38" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="123" t="s">
+      <c r="C38" s="103"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="101" t="s">
         <v>377</v>
       </c>
-      <c r="F38" s="115"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="115"/>
-      <c r="I38" s="115"/>
-      <c r="J38" s="115"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="115"/>
-      <c r="N38" s="115"/>
-      <c r="O38" s="115"/>
-      <c r="P38" s="115"/>
-      <c r="Q38" s="125"/>
-      <c r="R38" s="115"/>
-      <c r="S38" s="115"/>
-      <c r="T38" s="115"/>
-      <c r="U38" s="115"/>
-      <c r="V38" s="115"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="103"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="94"/>
+      <c r="O38" s="94"/>
+      <c r="P38" s="94"/>
+      <c r="Q38" s="103"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="94"/>
+      <c r="T38" s="94"/>
+      <c r="U38" s="94"/>
+      <c r="V38" s="94"/>
     </row>
     <row r="39" spans="1:22">
-      <c r="A39" s="124" t="s">
+      <c r="A39" s="102" t="s">
         <v>316</v>
       </c>
-      <c r="B39" s="122" t="s">
+      <c r="B39" s="100" t="s">
         <v>199</v>
       </c>
-      <c r="C39" s="125"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="123" t="s">
+      <c r="C39" s="103"/>
+      <c r="D39" s="103"/>
+      <c r="E39" s="101" t="s">
         <v>378</v>
       </c>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
-      <c r="H39" s="115"/>
-      <c r="I39" s="115"/>
-      <c r="J39" s="115"/>
-      <c r="K39" s="125"/>
-      <c r="L39" s="115"/>
-      <c r="M39" s="115"/>
-      <c r="N39" s="115"/>
-      <c r="O39" s="115"/>
-      <c r="P39" s="115"/>
-      <c r="Q39" s="125"/>
-      <c r="R39" s="115"/>
-      <c r="S39" s="115"/>
-      <c r="T39" s="115"/>
-      <c r="U39" s="115"/>
-      <c r="V39" s="115"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="94"/>
+      <c r="K39" s="103"/>
+      <c r="L39" s="94"/>
+      <c r="M39" s="94"/>
+      <c r="N39" s="94"/>
+      <c r="O39" s="94"/>
+      <c r="P39" s="94"/>
+      <c r="Q39" s="103"/>
+      <c r="R39" s="94"/>
+      <c r="S39" s="94"/>
+      <c r="T39" s="94"/>
+      <c r="U39" s="94"/>
+      <c r="V39" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="L3:P3"/>
     <mergeCell ref="R3:U3"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="L3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="R6:V9 F7:J9 L6:P9 R11:U12 L11:P12 F11:J12 B5:B19">
     <cfRule type="cellIs" dxfId="83" priority="345" operator="equal">
@@ -8351,7 +8348,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="12" customHeight="1" thickBot="1">
-      <c r="A4" s="93">
+      <c r="A4" s="107">
         <f>COUNTA(A6:A296)</f>
         <v>10</v>
       </c>
@@ -8377,7 +8374,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" thickBot="1">
-      <c r="A5" s="93"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="75"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -12927,7 +12924,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12948,18 +12945,18 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="118" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="E2" s="104" t="s">
+      <c r="C2" s="119"/>
+      <c r="E2" s="118" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="H2" s="104" t="s">
+      <c r="F2" s="119"/>
+      <c r="H2" s="118" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="105"/>
+      <c r="I2" s="119"/>
       <c r="K2" s="83" t="s">
         <v>359</v>
       </c>
@@ -13176,7 +13173,7 @@
   <dimension ref="A1:ALK293"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -13208,11 +13205,11 @@
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="M1" s="94" t="str">
+      <c r="M1" s="108" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="95"/>
+      <c r="N1" s="109"/>
     </row>
     <row r="2" spans="1:999" ht="18" customHeight="1">
       <c r="A2" s="38"/>
@@ -13230,11 +13227,11 @@
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="M2" s="94" t="str">
+      <c r="M2" s="108" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="95"/>
+      <c r="N2" s="109"/>
     </row>
     <row r="3" spans="1:999" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -13285,7 +13282,7 @@
     </row>
     <row r="4" spans="1:999" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B293)</f>
         <v>57</v>
       </c>
@@ -13328,7 +13325,7 @@
     </row>
     <row r="5" spans="1:999" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -13425,7 +13422,7 @@
       <c r="M7" s="33" t="s">
         <v>400</v>
       </c>
-      <c r="N7" s="107" t="s">
+      <c r="N7" s="33" t="s">
         <v>404</v>
       </c>
     </row>
@@ -13458,7 +13455,7 @@
       <c r="M8" s="33" t="s">
         <v>401</v>
       </c>
-      <c r="N8" s="107" t="s">
+      <c r="N8" s="33" t="s">
         <v>404</v>
       </c>
     </row>
@@ -13491,7 +13488,7 @@
       <c r="M9" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="N9" s="107" t="s">
+      <c r="N9" s="33" t="s">
         <v>404</v>
       </c>
     </row>
@@ -13524,7 +13521,7 @@
       <c r="M10" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="N10" s="107" t="s">
+      <c r="N10" s="33" t="s">
         <v>404</v>
       </c>
     </row>
@@ -19587,7 +19584,7 @@
     </row>
     <row r="4" spans="1:1009" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B300)</f>
         <v>14</v>
       </c>
@@ -19620,7 +19617,7 @@
     </row>
     <row r="5" spans="1:1009" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -24993,7 +24990,7 @@
     </row>
     <row r="4" spans="1:9" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B303)</f>
         <v>17</v>
       </c>
@@ -25019,7 +25016,7 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -28623,7 +28620,7 @@
     </row>
     <row r="4" spans="1:10" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B300)</f>
         <v>1</v>
       </c>
@@ -28653,7 +28650,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -32339,16 +32336,16 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
-      <c r="J1" s="96" t="str">
+      <c r="J1" s="110" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="94" t="str">
+      <c r="K1" s="110"/>
+      <c r="L1" s="108" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="95"/>
+      <c r="M1" s="109"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="39"/>
@@ -32360,16 +32357,16 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
-      <c r="J2" s="96" t="str">
+      <c r="J2" s="110" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="94" t="str">
+      <c r="K2" s="110"/>
+      <c r="L2" s="108" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="95"/>
+      <c r="M2" s="109"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -32414,7 +32411,7 @@
     </row>
     <row r="4" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B300)</f>
         <v>18</v>
       </c>
@@ -32447,7 +32444,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -37348,16 +37345,16 @@
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
-      <c r="I1" s="96" t="str">
+      <c r="I1" s="110" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="J1" s="96"/>
-      <c r="K1" s="94" t="str">
+      <c r="J1" s="110"/>
+      <c r="K1" s="108" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="L1" s="95"/>
+      <c r="L1" s="109"/>
     </row>
     <row r="2" spans="1:1019" ht="18" customHeight="1">
       <c r="A2" s="22"/>
@@ -37368,16 +37365,16 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
-      <c r="I2" s="96" t="str">
+      <c r="I2" s="110" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="J2" s="96"/>
-      <c r="K2" s="94" t="str">
+      <c r="J2" s="110"/>
+      <c r="K2" s="108" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="L2" s="95"/>
+      <c r="L2" s="109"/>
     </row>
     <row r="3" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -37420,7 +37417,7 @@
     </row>
     <row r="4" spans="1:1019" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B300)</f>
         <v>42</v>
       </c>
@@ -37450,7 +37447,7 @@
     </row>
     <row r="5" spans="1:1019" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -42226,16 +42223,16 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
-      <c r="K1" s="96" t="str">
+      <c r="K1" s="110" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="L1" s="96"/>
-      <c r="M1" s="94" t="str">
+      <c r="L1" s="110"/>
+      <c r="M1" s="108" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="N1" s="95"/>
+      <c r="N1" s="109"/>
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
     </row>
@@ -42250,16 +42247,16 @@
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
-      <c r="K2" s="96" t="str">
+      <c r="K2" s="110" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="94" t="str">
+      <c r="L2" s="110"/>
+      <c r="M2" s="108" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="N2" s="95"/>
+      <c r="N2" s="109"/>
       <c r="O2" s="39"/>
       <c r="P2" s="39"/>
     </row>
@@ -42303,15 +42300,15 @@
       <c r="M3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="97" t="s">
+      <c r="N3" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
     </row>
     <row r="4" spans="1:16" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B299)</f>
         <v>12</v>
       </c>
@@ -42347,7 +42344,7 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>
@@ -47908,16 +47905,16 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
-      <c r="J1" s="96" t="str">
+      <c r="J1" s="110" t="str">
         <f>proj_nr_descr</f>
         <v>Projectnumber:</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="94" t="str">
+      <c r="K1" s="110"/>
+      <c r="L1" s="108" t="str">
         <f>proj_nr</f>
         <v>[Enter proj nr]</v>
       </c>
-      <c r="M1" s="95"/>
+      <c r="M1" s="109"/>
     </row>
     <row r="2" spans="1:13" s="24" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="39"/>
@@ -47929,16 +47926,16 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
-      <c r="J2" s="96" t="str">
+      <c r="J2" s="110" t="str">
         <f>proj_name_descr</f>
         <v>Projectname:</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="94" t="str">
+      <c r="K2" s="110"/>
+      <c r="L2" s="108" t="str">
         <f>proj_name</f>
         <v>[Enter proj name]</v>
       </c>
-      <c r="M2" s="95"/>
+      <c r="M2" s="109"/>
     </row>
     <row r="3" spans="1:13" s="24" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="23" t="s">
@@ -47983,7 +47980,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1">
       <c r="A4" s="25"/>
-      <c r="B4" s="93">
+      <c r="B4" s="107">
         <f>COUNTA(B6:B300)</f>
         <v>7</v>
       </c>
@@ -48013,7 +48010,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="A5" s="29"/>
-      <c r="B5" s="93"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="30"/>

</xml_diff>